<commit_message>
updating inputs and information to align with version 5.0 of Briggs excel tool
</commit_message>
<xml_diff>
--- a/Inputs/inputs.xlsx
+++ b/Inputs/inputs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eidennay\Documents\Other\general\covid19_QALY_calculator\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eidennay\Documents\LSHTM\covid19\COVID19_QALY_App\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6180" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6180" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="male_LT" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -148,7 +148,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2886,8 +2886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="H111" sqref="H111"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5341,8 +5341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5442,7 +5442,7 @@
         <v>0.91200000000000003</v>
       </c>
       <c r="F4">
-        <v>0.96</v>
+        <v>0.88100000000000001</v>
       </c>
       <c r="G4">
         <v>0.87</v>
@@ -5468,7 +5468,7 @@
         <v>0.88900000000000001</v>
       </c>
       <c r="F5">
-        <v>0.94399999999999995</v>
+        <v>0.878</v>
       </c>
       <c r="G5">
         <v>0.85</v>
@@ -5494,7 +5494,7 @@
         <v>0.85499999999999998</v>
       </c>
       <c r="F6">
-        <v>0.90500000000000003</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="G6">
         <v>0.82</v>
@@ -5520,7 +5520,7 @@
         <v>0.83</v>
       </c>
       <c r="F7">
-        <v>0.93700000000000006</v>
+        <v>0.83899999999999997</v>
       </c>
       <c r="G7">
         <v>0.8</v>
@@ -5546,7 +5546,7 @@
         <v>0.81699999999999995</v>
       </c>
       <c r="F8">
-        <v>0.93100000000000005</v>
+        <v>0.86699999999999999</v>
       </c>
       <c r="G8">
         <v>0.8</v>
@@ -5572,7 +5572,7 @@
         <v>0.755</v>
       </c>
       <c r="F9">
-        <v>0.86799999999999999</v>
+        <v>0.86099999999999999</v>
       </c>
       <c r="G9">
         <v>0.76</v>
@@ -5590,8 +5590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5633,19 +5633,19 @@
         <v>9</v>
       </c>
       <c r="D2" s="1">
-        <v>4.4740727484228892E-5</v>
+        <v>6.0475336142076724E-5</v>
       </c>
       <c r="E2">
-        <v>2.2161015607686708E-4</v>
+        <v>1.9603300482954038E-4</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1.1305822354073918E-4</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>9.3023255813953494E-4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -5659,19 +5659,19 @@
         <v>19</v>
       </c>
       <c r="D3" s="1">
-        <v>3.5792581987383114E-4</v>
+        <v>2.419013445683069E-4</v>
       </c>
       <c r="E3">
-        <v>5.5402539019216762E-4</v>
+        <v>6.950261080320068E-4</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1.2782162073571416E-8</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1.8604651162790699E-3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -5685,19 +5685,19 @@
         <v>29</v>
       </c>
       <c r="D4" s="1">
-        <v>1.7001476444006979E-3</v>
+        <v>1.4715665127905337E-3</v>
       </c>
       <c r="E4">
-        <v>4.3530566372241746E-3</v>
+        <v>4.0632295546486558E-3</v>
       </c>
       <c r="F4">
-        <v>2.9420417769932335E-3</v>
+        <v>1.0175240118666525E-3</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>2.7906976744186047E-3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -5711,19 +5711,19 @@
         <v>39</v>
       </c>
       <c r="D5" s="1">
-        <v>4.9214800232651786E-3</v>
+        <v>4.1526397484226013E-3</v>
       </c>
       <c r="E5">
-        <v>1.3312438661474657E-2</v>
+        <v>1.2216420437331812E-2</v>
       </c>
       <c r="F5">
-        <v>5.884083553986467E-3</v>
+        <v>1.6958733531110878E-3</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>9.433962264150943E-3</v>
+        <v>3.7209302325581397E-3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -5737,19 +5737,19 @@
         <v>49</v>
       </c>
       <c r="D6" s="1">
-        <v>1.619614334929086E-2</v>
+        <v>1.3909327312677647E-2</v>
       </c>
       <c r="E6">
-        <v>3.5584259347199797E-2</v>
+        <v>3.323650490973571E-2</v>
       </c>
       <c r="F6">
-        <v>1.4416004707266842E-2</v>
+        <v>5.3137365064147412E-3</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1.984126984126984E-2</v>
       </c>
       <c r="H6">
-        <v>9.433962264150943E-3</v>
+        <v>1.3023255813953489E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -5763,19 +5763,19 @@
         <v>59</v>
       </c>
       <c r="D7" s="1">
-        <v>5.2928280613842783E-2</v>
+        <v>4.5719354123410001E-2</v>
       </c>
       <c r="E7">
-        <v>8.8944819071136855E-2</v>
+        <v>8.4441216830324517E-2</v>
       </c>
       <c r="F7">
-        <v>2.8832009414533684E-2</v>
+        <v>2.340305227293301E-2</v>
       </c>
       <c r="G7">
-        <v>3.5502958579881658E-2</v>
+        <v>2.3809523809523808E-2</v>
       </c>
       <c r="H7">
-        <v>3.3018867924528301E-2</v>
+        <v>4.3720930232558138E-2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -5789,19 +5789,19 @@
         <v>69</v>
       </c>
       <c r="D8" s="1">
-        <v>0.11475996599704712</v>
+        <v>9.6679904045799986E-2</v>
       </c>
       <c r="E8">
-        <v>0.17113052838192927</v>
+        <v>0.16394596617539609</v>
       </c>
       <c r="F8">
-        <v>9.3262724330685498E-2</v>
+        <v>7.1452797277747157E-2</v>
       </c>
       <c r="G8">
-        <v>5.9171597633136092E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="H8">
-        <v>9.9056603773584911E-2</v>
+        <v>0.10232558139534884</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -5815,19 +5815,19 @@
         <v>79</v>
       </c>
       <c r="D9" s="1">
-        <v>0.24929533354212338</v>
+        <v>0.22504888423004818</v>
       </c>
       <c r="E9">
-        <v>0.24453097793396017</v>
+        <v>0.23663411330707679</v>
       </c>
       <c r="F9">
-        <v>0.186525448661371</v>
+        <v>0.18111927411226417</v>
       </c>
       <c r="G9">
-        <v>0.22485207100591717</v>
+        <v>0.23412698412698413</v>
       </c>
       <c r="H9">
-        <v>0.23584905660377359</v>
+        <v>0.23069767441860464</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -5841,19 +5841,19 @@
         <v>89</v>
       </c>
       <c r="D10" s="1">
-        <v>0.38092255380072482</v>
+        <v>0.39520632168847136</v>
       </c>
       <c r="E10">
-        <v>0.2888055212587457</v>
+        <v>0.29862509578885466</v>
       </c>
       <c r="F10">
-        <v>0.44542512503677556</v>
+        <v>0.35794233572998024</v>
       </c>
       <c r="G10">
-        <v>0.378698224852071</v>
+        <v>0.34920634920634919</v>
       </c>
       <c r="H10">
-        <v>0.30188679245283018</v>
+        <v>0.35627906976744184</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -5867,19 +5867,19 @@
         <v>100</v>
       </c>
       <c r="D11" s="1">
-        <v>0.17887342848194712</v>
+        <v>0.21750962565766929</v>
       </c>
       <c r="E11">
-        <v>0.15256276316206033</v>
+        <v>0.16594639388377025</v>
       </c>
       <c r="F11">
-        <v>0.22271256251838778</v>
+        <v>0.35794233572998024</v>
       </c>
       <c r="G11">
-        <v>0.30177514792899407</v>
+        <v>0.28968253968253971</v>
       </c>
       <c r="H11">
-        <v>0.31132075471698112</v>
+        <v>0.24465116279069768</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating and checking decimal place values copied over from excel tool into input.xlsx
</commit_message>
<xml_diff>
--- a/Inputs/inputs.xlsx
+++ b/Inputs/inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6180" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6180" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="male_LT" sheetId="1" r:id="rId1"/>
@@ -114,8 +114,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="170" formatCode="0.0000000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -146,9 +147,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +434,14 @@
   <dimension ref="A1:F122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -471,7 +477,7 @@
         <v>4.7699999999999999E-3</v>
       </c>
       <c r="E2">
-        <v>2E-3</v>
+        <v>2.4320000000000001E-3</v>
       </c>
       <c r="F2">
         <v>3.3355012147736913E-3</v>
@@ -491,7 +497,7 @@
         <v>2.7999999999999998E-4</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>2.3900000000000001E-4</v>
       </c>
       <c r="F3">
         <v>3.0488727551586457E-4</v>
@@ -511,7 +517,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1.64E-4</v>
       </c>
       <c r="F4">
         <v>2.2728948922868928E-4</v>
@@ -531,7 +537,7 @@
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>6.3999999999999997E-5</v>
       </c>
       <c r="F5">
         <v>1.7559773686957376E-4</v>
@@ -551,7 +557,7 @@
         <v>1.2E-4</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1.2799999999999999E-4</v>
       </c>
       <c r="F6">
         <v>1.4098471058326208E-4</v>
@@ -571,7 +577,7 @@
         <v>1E-4</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1.2799999999999999E-4</v>
       </c>
       <c r="F7">
         <v>1.17964870067062E-4</v>
@@ -591,7 +597,7 @@
         <v>9.0000000000000006E-5</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>3.1000000000000001E-5</v>
       </c>
       <c r="F8">
         <v>1.0315136436683143E-4</v>
@@ -611,7 +617,7 @@
         <v>8.0000000000000007E-5</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1.2300000000000001E-4</v>
       </c>
       <c r="F9">
         <v>9.4526352235802316E-5</v>
@@ -651,7 +657,7 @@
         <v>8.0000000000000007E-5</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1.47E-4</v>
       </c>
       <c r="F11">
         <v>9.239145173632458E-5</v>
@@ -691,7 +697,7 @@
         <v>1E-4</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="F13">
         <v>1.1075497099642469E-4</v>
@@ -711,7 +717,7 @@
         <v>1.1E-4</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1.8200000000000001E-4</v>
       </c>
       <c r="F14">
         <v>1.2852899894834206E-4</v>
@@ -731,7 +737,7 @@
         <v>1.3999999999999999E-4</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>9.2E-5</v>
       </c>
       <c r="F15">
         <v>1.5302678270302865E-4</v>
@@ -751,7 +757,7 @@
         <v>1.8000000000000001E-4</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>6.2000000000000003E-5</v>
       </c>
       <c r="F16">
         <v>1.8508551197572555E-4</v>
@@ -771,7 +777,7 @@
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>2.4800000000000001E-4</v>
       </c>
       <c r="F17">
         <v>2.2517817009709014E-4</v>
@@ -791,7 +797,7 @@
         <v>3.3E-4</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>2.5099999999999998E-4</v>
       </c>
       <c r="F18">
         <v>2.7285961352202601E-4</v>
@@ -811,7 +817,7 @@
         <v>4.2000000000000002E-4</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>2.4899999999999998E-4</v>
       </c>
       <c r="F19">
         <v>3.2607805838455928E-4</v>
@@ -831,7 +837,7 @@
         <v>5.1000000000000004E-4</v>
       </c>
       <c r="E20">
-        <v>1E-3</v>
+        <v>5.3700000000000004E-4</v>
       </c>
       <c r="F20">
         <v>3.8052523684085573E-4</v>
@@ -851,7 +857,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>4.9100000000000001E-4</v>
       </c>
       <c r="F21">
         <v>4.3035497695416989E-4</v>
@@ -871,7 +877,7 @@
         <v>6.8000000000000005E-4</v>
       </c>
       <c r="E22">
-        <v>1E-3</v>
+        <v>6.9700000000000003E-4</v>
       </c>
       <c r="F22">
         <v>4.7241129835084056E-4</v>
@@ -891,7 +897,7 @@
         <v>7.5000000000000002E-4</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>3.19E-4</v>
       </c>
       <c r="F23">
         <v>5.0527066256768414E-4</v>
@@ -911,7 +917,7 @@
         <v>8.0999999999999996E-4</v>
       </c>
       <c r="E24">
-        <v>1E-3</v>
+        <v>5.3600000000000002E-4</v>
       </c>
       <c r="F24">
         <v>5.2856515581709658E-4</v>
@@ -931,7 +937,7 @@
         <v>8.5999999999999998E-4</v>
       </c>
       <c r="E25">
-        <v>1E-3</v>
+        <v>6.3900000000000003E-4</v>
       </c>
       <c r="F25">
         <v>5.4288006965963226E-4</v>
@@ -951,7 +957,7 @@
         <v>8.8000000000000003E-4</v>
       </c>
       <c r="E26">
-        <v>1E-3</v>
+        <v>8.3199999999999995E-4</v>
       </c>
       <c r="F26">
         <v>5.495414638213925E-4</v>
@@ -971,7 +977,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="E27">
-        <v>1E-3</v>
+        <v>6.0499999999999996E-4</v>
       </c>
       <c r="F27">
         <v>5.5036209419761443E-4</v>
@@ -991,7 +997,7 @@
         <v>9.2000000000000003E-4</v>
       </c>
       <c r="E28">
-        <v>1E-3</v>
+        <v>6.7100000000000005E-4</v>
       </c>
       <c r="F28">
         <v>5.4740444888810456E-4</v>
@@ -1011,7 +1017,7 @@
         <v>9.3999999999999997E-4</v>
       </c>
       <c r="E29">
-        <v>1E-3</v>
+        <v>5.7499999999999999E-4</v>
       </c>
       <c r="F29">
         <v>5.4280041442391952E-4</v>
@@ -1031,7 +1037,7 @@
         <v>9.7000000000000005E-4</v>
       </c>
       <c r="E30">
-        <v>1E-3</v>
+        <v>6.96E-4</v>
       </c>
       <c r="F30">
         <v>5.3864711478353105E-4</v>
@@ -1051,7 +1057,7 @@
         <v>1E-3</v>
       </c>
       <c r="E31">
-        <v>1E-3</v>
+        <v>6.1499999999999999E-4</v>
       </c>
       <c r="F31">
         <v>5.3698370195766581E-4</v>
@@ -1071,7 +1077,7 @@
         <v>1.0300000000000001E-3</v>
       </c>
       <c r="E32">
-        <v>1E-3</v>
+        <v>6.1799999999999995E-4</v>
       </c>
       <c r="F32">
         <v>5.3984707218313575E-4</v>
@@ -1091,7 +1097,7 @@
         <v>1.07E-3</v>
       </c>
       <c r="E33">
-        <v>1E-3</v>
+        <v>5.7799999999999995E-4</v>
       </c>
       <c r="F33">
         <v>5.489860358371399E-4</v>
@@ -1111,7 +1117,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="E34">
-        <v>1E-3</v>
+        <v>6.9300000000000004E-4</v>
       </c>
       <c r="F34">
         <v>5.6471814225685058E-4</v>
@@ -1131,7 +1137,7 @@
         <v>1.1299999999999999E-3</v>
       </c>
       <c r="E35">
-        <v>1E-3</v>
+        <v>5.0799999999999999E-4</v>
       </c>
       <c r="F35">
         <v>5.8714966012145926E-4</v>
@@ -1151,7 +1157,7 @@
         <v>1.15E-3</v>
       </c>
       <c r="E36">
-        <v>1E-3</v>
+        <v>5.9599999999999996E-4</v>
       </c>
       <c r="F36">
         <v>6.1656554924090559E-4</v>
@@ -1171,7 +1177,7 @@
         <v>1.16E-3</v>
       </c>
       <c r="E37">
-        <v>1E-3</v>
+        <v>6.8099999999999996E-4</v>
       </c>
       <c r="F37">
         <v>6.534160517827751E-4</v>
@@ -1191,7 +1197,7 @@
         <v>1.1800000000000001E-3</v>
       </c>
       <c r="E38">
-        <v>1E-3</v>
+        <v>7.8600000000000002E-4</v>
       </c>
       <c r="F38">
         <v>6.98308266286461E-4</v>
@@ -1211,7 +1217,7 @@
         <v>1.2099999999999999E-3</v>
       </c>
       <c r="E39">
-        <v>1E-3</v>
+        <v>9.3499999999999996E-4</v>
       </c>
       <c r="F39">
         <v>7.5200052315480112E-4</v>
@@ -1231,7 +1237,7 @@
         <v>1.2600000000000001E-3</v>
       </c>
       <c r="E40">
-        <v>1E-3</v>
+        <v>8.8400000000000002E-4</v>
       </c>
       <c r="F40">
         <v>8.153975725440503E-4</v>
@@ -1251,7 +1257,7 @@
         <v>1.32E-3</v>
       </c>
       <c r="E41">
-        <v>1E-3</v>
+        <v>9.3599999999999998E-4</v>
       </c>
       <c r="F41">
         <v>8.8954461238466883E-4</v>
@@ -1271,7 +1277,7 @@
         <v>1.4E-3</v>
       </c>
       <c r="E42">
-        <v>1E-3</v>
+        <v>1.1130000000000001E-3</v>
       </c>
       <c r="F42">
         <v>9.756180738139822E-4</v>
@@ -1291,7 +1297,7 @@
         <v>1.5E-3</v>
       </c>
       <c r="E43">
-        <v>1E-3</v>
+        <v>7.9500000000000003E-4</v>
       </c>
       <c r="F43">
         <v>1.0749108856967801E-3</v>
@@ -1311,7 +1317,7 @@
         <v>1.6000000000000001E-3</v>
       </c>
       <c r="E44">
-        <v>1E-3</v>
+        <v>9.3800000000000003E-4</v>
       </c>
       <c r="F44">
         <v>1.1888097032346889E-3</v>
@@ -1331,7 +1337,7 @@
         <v>1.72E-3</v>
       </c>
       <c r="E45">
-        <v>1E-3</v>
+        <v>1.444E-3</v>
       </c>
       <c r="F45">
         <v>1.3187613604175336E-3</v>
@@ -1351,7 +1357,7 @@
         <v>1.8400000000000001E-3</v>
       </c>
       <c r="E46">
-        <v>1E-3</v>
+        <v>1.351E-3</v>
       </c>
       <c r="F46">
         <v>1.4662256582004076E-3</v>
@@ -1371,7 +1377,7 @@
         <v>1.98E-3</v>
       </c>
       <c r="E47">
-        <v>1E-3</v>
+        <v>1.1069999999999999E-3</v>
       </c>
       <c r="F47">
         <v>1.6326116124622475E-3</v>
@@ -1391,7 +1397,7 @@
         <v>2.14E-3</v>
       </c>
       <c r="E48">
-        <v>2E-3</v>
+        <v>1.6280000000000001E-3</v>
       </c>
       <c r="F48">
         <v>1.8191945580248307E-3</v>
@@ -1411,7 +1417,7 @@
         <v>2.31E-3</v>
       </c>
       <c r="E49">
-        <v>2E-3</v>
+        <v>1.5839999999999999E-3</v>
       </c>
       <c r="F49">
         <v>2.0270121513730728E-3</v>
@@ -1431,7 +1437,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="E50">
-        <v>2E-3</v>
+        <v>1.57E-3</v>
       </c>
       <c r="F50">
         <v>2.2567384547136082E-3</v>
@@ -1451,7 +1457,7 @@
         <v>2.7100000000000002E-3</v>
       </c>
       <c r="E51">
-        <v>2E-3</v>
+        <v>1.616E-3</v>
       </c>
       <c r="F51">
         <v>2.5085370269668896E-3</v>
@@ -1471,7 +1477,7 @@
         <v>2.9499999999999999E-3</v>
       </c>
       <c r="E52">
-        <v>2E-3</v>
+        <v>1.9419999999999999E-3</v>
       </c>
       <c r="F52">
         <v>2.7818963688663709E-3</v>
@@ -1491,7 +1497,7 @@
         <v>3.2100000000000002E-3</v>
       </c>
       <c r="E53">
-        <v>2E-3</v>
+        <v>2.2669999999999999E-3</v>
       </c>
       <c r="F53">
         <v>3.0760282854001039E-3</v>
@@ -1511,7 +1517,7 @@
         <v>3.49E-3</v>
       </c>
       <c r="E54">
-        <v>3.0000000000000001E-3</v>
+        <v>2.5899999999999999E-3</v>
       </c>
       <c r="F54">
         <v>3.391881733747337E-3</v>
@@ -1531,7 +1537,7 @@
         <v>3.81E-3</v>
       </c>
       <c r="E55">
-        <v>3.0000000000000001E-3</v>
+        <v>2.5869999999999999E-3</v>
       </c>
       <c r="F55">
         <v>3.7311713566887555E-3</v>
@@ -1551,7 +1557,7 @@
         <v>4.15E-3</v>
       </c>
       <c r="E56">
-        <v>3.0000000000000001E-3</v>
+        <v>3.2659999999999998E-3</v>
       </c>
       <c r="F56">
         <v>4.0959714753958272E-3</v>
@@ -1571,7 +1577,7 @@
         <v>4.5300000000000002E-3</v>
       </c>
       <c r="E57">
-        <v>3.0000000000000001E-3</v>
+        <v>3.3890000000000001E-3</v>
       </c>
       <c r="F57">
         <v>4.4887870748620048E-3</v>
@@ -1591,7 +1597,7 @@
         <v>4.9399999999999999E-3</v>
       </c>
       <c r="E58">
-        <v>4.0000000000000001E-3</v>
+        <v>4.0429999999999997E-3</v>
       </c>
       <c r="F58">
         <v>4.9126356736124031E-3</v>
@@ -1611,7 +1617,7 @@
         <v>5.4000000000000003E-3</v>
       </c>
       <c r="E59">
-        <v>5.0000000000000001E-3</v>
+        <v>4.5840000000000004E-3</v>
       </c>
       <c r="F59">
         <v>5.3711427957865224E-3</v>
@@ -1631,7 +1637,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
       <c r="E60">
-        <v>4.0000000000000001E-3</v>
+        <v>4.215E-3</v>
       </c>
       <c r="F60">
         <v>5.8686545478524223E-3</v>
@@ -1651,7 +1657,7 @@
         <v>6.4599999999999996E-3</v>
       </c>
       <c r="E61">
-        <v>5.0000000000000001E-3</v>
+        <v>5.4780000000000002E-3</v>
       </c>
       <c r="F61">
         <v>6.4103717768593856E-3</v>
@@ -1671,7 +1677,7 @@
         <v>7.0699999999999999E-3</v>
       </c>
       <c r="E62">
-        <v>6.0000000000000001E-3</v>
+        <v>5.7930000000000004E-3</v>
       </c>
       <c r="F62">
         <v>7.0025115114069605E-3</v>
@@ -1691,7 +1697,7 @@
         <v>7.7400000000000004E-3</v>
       </c>
       <c r="E63">
-        <v>7.0000000000000001E-3</v>
+        <v>6.6439999999999997E-3</v>
       </c>
       <c r="F63">
         <v>7.6525029404624122E-3</v>
@@ -1711,7 +1717,7 @@
         <v>8.4799999999999997E-3</v>
       </c>
       <c r="E64">
-        <v>8.0000000000000002E-3</v>
+        <v>7.5380000000000004E-3</v>
       </c>
       <c r="F64">
         <v>8.369227176811888E-3</v>
@@ -1731,7 +1737,7 @@
         <v>9.2999999999999992E-3</v>
       </c>
       <c r="E65">
-        <v>8.9999999999999993E-3</v>
+        <v>8.6370000000000006E-3</v>
       </c>
       <c r="F65">
         <v>9.163312626898467E-3</v>
@@ -1751,7 +1757,7 @@
         <v>1.021E-2</v>
       </c>
       <c r="E66">
-        <v>8.0000000000000002E-3</v>
+        <v>8.4770000000000002E-3</v>
       </c>
       <c r="F66">
         <v>1.0047501143829948E-2</v>
@@ -1771,7 +1777,7 @@
         <v>1.1209999999999999E-2</v>
       </c>
       <c r="E67">
-        <v>0.01</v>
+        <v>1.0345E-2</v>
       </c>
       <c r="F67">
         <v>1.1037104542155392E-2</v>
@@ -1791,7 +1797,7 @@
         <v>1.231E-2</v>
       </c>
       <c r="E68">
-        <v>0.01</v>
+        <v>1.0154E-2</v>
       </c>
       <c r="F68">
         <v>1.214948031242649E-2</v>
@@ -1811,7 +1817,7 @@
         <v>1.354E-2</v>
       </c>
       <c r="E69">
-        <v>1.0999999999999999E-2</v>
+        <v>1.1258000000000001E-2</v>
       </c>
       <c r="F69">
         <v>1.340055670787192E-2</v>
@@ -1831,7 +1837,7 @@
         <v>1.49E-2</v>
       </c>
       <c r="E70">
-        <v>1.2E-2</v>
+        <v>1.1787000000000001E-2</v>
       </c>
       <c r="F70">
         <v>1.4807049176730036E-2</v>
@@ -1851,7 +1857,7 @@
         <v>1.6400000000000001E-2</v>
       </c>
       <c r="E71">
-        <v>1.4999999999999999E-2</v>
+        <v>1.481E-2</v>
       </c>
       <c r="F71">
         <v>1.6387499062380829E-2</v>
@@ -1871,7 +1877,7 @@
         <v>1.8069999999999999E-2</v>
       </c>
       <c r="E72">
-        <v>1.4999999999999999E-2</v>
+        <v>1.5487000000000001E-2</v>
       </c>
       <c r="F72">
         <v>1.8162401370356733E-2</v>
@@ -1891,7 +1897,7 @@
         <v>1.992E-2</v>
       </c>
       <c r="E73">
-        <v>1.7999999999999999E-2</v>
+        <v>1.8338E-2</v>
       </c>
       <c r="F73">
         <v>2.0154323751890971E-2</v>
@@ -1911,7 +1917,7 @@
         <v>2.197E-2</v>
       </c>
       <c r="E74">
-        <v>1.9E-2</v>
+        <v>1.8721999999999999E-2</v>
       </c>
       <c r="F74">
         <v>2.2388010903042245E-2</v>
@@ -1931,7 +1937,7 @@
         <v>2.4250000000000001E-2</v>
       </c>
       <c r="E75">
-        <v>2.1999999999999999E-2</v>
+        <v>2.2290000000000001E-2</v>
       </c>
       <c r="F75">
         <v>2.489046733936006E-2</v>
@@ -1951,7 +1957,7 @@
         <v>2.6790000000000001E-2</v>
       </c>
       <c r="E76">
-        <v>2.4E-2</v>
+        <v>2.4058E-2</v>
       </c>
       <c r="F76">
         <v>2.7691010156181042E-2</v>
@@ -1971,7 +1977,7 @@
         <v>2.9610000000000001E-2</v>
       </c>
       <c r="E77">
-        <v>2.9000000000000001E-2</v>
+        <v>2.8884E-2</v>
       </c>
       <c r="F77">
         <v>3.0821281951554983E-2</v>
@@ -1991,7 +1997,7 @@
         <v>3.2750000000000001E-2</v>
       </c>
       <c r="E78">
-        <v>2.9000000000000001E-2</v>
+        <v>2.9142999999999999E-2</v>
       </c>
       <c r="F78">
         <v>3.4315212614492795E-2</v>
@@ -2011,7 +2017,7 @@
         <v>3.6240000000000001E-2</v>
       </c>
       <c r="E79">
-        <v>3.3000000000000002E-2</v>
+        <v>3.3099000000000003E-2</v>
       </c>
       <c r="F79">
         <v>3.8208917224974118E-2</v>
@@ -2031,7 +2037,7 @@
         <v>4.0129999999999999E-2</v>
       </c>
       <c r="E80">
-        <v>3.6999999999999998E-2</v>
+        <v>3.6643000000000002E-2</v>
       </c>
       <c r="F80">
         <v>4.25405159529334E-2</v>
@@ -2051,7 +2057,7 @@
         <v>4.4470000000000003E-2</v>
       </c>
       <c r="E81">
-        <v>4.2999999999999997E-2</v>
+        <v>4.3049999999999998E-2</v>
       </c>
       <c r="F81">
         <v>4.734986068227106E-2</v>
@@ -2071,7 +2077,7 @@
         <v>4.931E-2</v>
       </c>
       <c r="E82">
-        <v>4.5999999999999999E-2</v>
+        <v>4.5641000000000001E-2</v>
       </c>
       <c r="F82">
         <v>5.2678152247148315E-2</v>
@@ -2091,7 +2097,7 @@
         <v>5.4719999999999998E-2</v>
       </c>
       <c r="E83">
-        <v>5.3999999999999999E-2</v>
+        <v>5.4267000000000003E-2</v>
       </c>
       <c r="F83">
         <v>5.8567431799203533E-2</v>
@@ -2111,7 +2117,7 @@
         <v>6.0749999999999998E-2</v>
       </c>
       <c r="E84">
-        <v>5.8999999999999997E-2</v>
+        <v>5.8616000000000001E-2</v>
       </c>
       <c r="F84">
         <v>6.5059930095693483E-2</v>
@@ -2131,7 +2137,7 @@
         <v>6.7489999999999994E-2</v>
       </c>
       <c r="E85">
-        <v>7.5999999999999998E-2</v>
+        <v>7.5734999999999997E-2</v>
       </c>
       <c r="F85">
         <v>7.2197259597767807E-2</v>
@@ -2151,7 +2157,7 @@
         <v>7.5039999999999996E-2</v>
       </c>
       <c r="E86">
-        <v>7.9000000000000001E-2</v>
+        <v>7.9090999999999995E-2</v>
       </c>
       <c r="F86">
         <v>8.0019436394626844E-2</v>
@@ -2171,7 +2177,7 @@
         <v>8.3479999999999999E-2</v>
       </c>
       <c r="E87">
-        <v>9.0999999999999998E-2</v>
+        <v>9.1314999999999993E-2</v>
       </c>
       <c r="F87">
         <v>8.8563722324135605E-2</v>
@@ -2191,7 +2197,7 @@
         <v>9.2920000000000003E-2</v>
       </c>
       <c r="E88">
-        <v>0.1</v>
+        <v>9.9890000000000007E-2</v>
       </c>
       <c r="F88">
         <v>9.7863282432521209E-2</v>
@@ -2211,7 +2217,7 @@
         <v>0.10351</v>
       </c>
       <c r="E89">
-        <v>0.11799999999999999</v>
+        <v>0.117919</v>
       </c>
       <c r="F89">
         <v>0.10794565926430064</v>
@@ -2231,7 +2237,7 @@
         <v>0.11537</v>
       </c>
       <c r="E90">
-        <v>0.13700000000000001</v>
+        <v>0.13652400000000001</v>
       </c>
       <c r="F90">
         <v>0.11883107350657646</v>
@@ -2251,7 +2257,7 @@
         <v>0.12867999999999999</v>
       </c>
       <c r="E91">
-        <v>0.14099999999999999</v>
+        <v>0.141206</v>
       </c>
       <c r="F91">
         <v>0.13053057026155271</v>
@@ -2271,7 +2277,7 @@
         <v>0.14362</v>
       </c>
       <c r="E92">
-        <v>0.17</v>
+        <v>0.17013300000000001</v>
       </c>
       <c r="F92">
         <v>0.14304404161680509</v>
@@ -2291,7 +2297,7 @@
         <v>0.15998000000000001</v>
       </c>
       <c r="E93">
-        <v>0.187</v>
+        <v>0.18690699999999999</v>
       </c>
       <c r="F93">
         <v>0.1563614837270379</v>
@@ -2311,7 +2317,7 @@
         <v>0.1774</v>
       </c>
       <c r="E94">
-        <v>0.22</v>
+        <v>0.219579</v>
       </c>
       <c r="F94">
         <v>0.1704732516438846</v>
@@ -2331,7 +2337,7 @@
         <v>0.19581999999999999</v>
       </c>
       <c r="E95">
-        <v>0.22900000000000001</v>
+        <v>0.22897600000000001</v>
       </c>
       <c r="F95">
         <v>0.18536269877153885</v>
@@ -2351,7 +2357,7 @@
         <v>0.21517</v>
       </c>
       <c r="E96">
-        <v>0.25</v>
+        <v>0.25034499999999998</v>
       </c>
       <c r="F96">
         <v>0.20100240983568257</v>
@@ -2371,7 +2377,7 @@
         <v>0.23558000000000001</v>
       </c>
       <c r="E97">
-        <v>0.253</v>
+        <v>0.252776</v>
       </c>
       <c r="F97">
         <v>0.21735327631486584</v>
@@ -2391,7 +2397,7 @@
         <v>0.25607000000000002</v>
       </c>
       <c r="E98">
-        <v>0.26200000000000001</v>
+        <v>0.262409</v>
       </c>
       <c r="F98">
         <v>0.23436368016978865</v>
@@ -2411,7 +2417,7 @@
         <v>0.2772</v>
       </c>
       <c r="E99">
-        <v>0.33400000000000002</v>
+        <v>0.33420899999999998</v>
       </c>
       <c r="F99">
         <v>0.25196882065580722</v>
@@ -2431,7 +2437,7 @@
         <v>0.29880000000000001</v>
       </c>
       <c r="E100">
-        <v>0.313</v>
+        <v>0.312801</v>
       </c>
       <c r="F100">
         <v>0.27009021996976162</v>
@@ -2451,7 +2457,7 @@
         <v>0.32069999999999999</v>
       </c>
       <c r="E101">
-        <v>0.36599999999999999</v>
+        <v>0.36642400000000003</v>
       </c>
       <c r="F101">
         <v>0.28863544340130187</v>
@@ -2471,7 +2477,7 @@
         <v>0.34271000000000001</v>
       </c>
       <c r="E102">
-        <v>0.33500000000000002</v>
+        <v>0.33546599999999999</v>
       </c>
       <c r="F102">
         <v>0.30749806836814941</v>
@@ -2887,10 +2893,15 @@
   <dimension ref="A1:F122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -2926,7 +2937,7 @@
         <v>4.2700000000000004E-3</v>
       </c>
       <c r="E2">
-        <v>2E-3</v>
+        <v>1.6850000000000001E-3</v>
       </c>
       <c r="F2">
         <v>2.9369651296826337E-3</v>
@@ -2946,7 +2957,7 @@
         <v>2.3000000000000001E-4</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1.45E-4</v>
       </c>
       <c r="F3">
         <v>2.7644384434394743E-4</v>
@@ -2966,7 +2977,7 @@
         <v>1.7000000000000001E-4</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>6.9999999999999994E-5</v>
       </c>
       <c r="F4">
         <v>1.7711147643617917E-4</v>
@@ -2986,7 +2997,7 @@
         <v>1.2999999999999999E-4</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>6.7999999999999999E-5</v>
       </c>
       <c r="F5">
         <v>1.266238663112896E-4</v>
@@ -3006,7 +3017,7 @@
         <v>1.1E-4</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1.01E-4</v>
       </c>
       <c r="F6">
         <v>9.9624459829725763E-5</v>
@@ -3046,7 +3057,7 @@
         <v>8.0000000000000007E-5</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>6.6000000000000005E-5</v>
       </c>
       <c r="F8">
         <v>7.7735832045600889E-5</v>
@@ -3086,7 +3097,7 @@
         <v>6.9999999999999994E-5</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>9.5000000000000005E-5</v>
       </c>
       <c r="F10">
         <v>7.5271776536278291E-5</v>
@@ -3106,7 +3117,7 @@
         <v>6.9999999999999994E-5</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>6.2000000000000003E-5</v>
       </c>
       <c r="F11">
         <v>7.756702406156658E-5</v>
@@ -3126,7 +3137,7 @@
         <v>8.0000000000000007E-5</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>9.2999999999999997E-5</v>
       </c>
       <c r="F12">
         <v>8.107307695627859E-5</v>
@@ -3146,7 +3157,7 @@
         <v>8.0000000000000007E-5</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>6.3E-5</v>
       </c>
       <c r="F13">
         <v>8.5600169335157232E-5</v>
@@ -3166,7 +3177,7 @@
         <v>9.0000000000000006E-5</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="F14">
         <v>9.1111499780282821E-5</v>
@@ -3206,7 +3217,7 @@
         <v>1.2999999999999999E-4</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1.6200000000000001E-4</v>
       </c>
       <c r="F16">
         <v>1.0487713192131304E-4</v>
@@ -3226,7 +3237,7 @@
         <v>1.6000000000000001E-4</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1.2999999999999999E-4</v>
       </c>
       <c r="F17">
         <v>1.1295206169620873E-4</v>
@@ -3246,7 +3257,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1.3100000000000001E-4</v>
       </c>
       <c r="F18">
         <v>1.2162329851986952E-4</v>
@@ -3266,7 +3277,7 @@
         <v>2.4000000000000001E-4</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>6.6000000000000005E-5</v>
       </c>
       <c r="F19">
         <v>1.3066245400610618E-4</v>
@@ -3286,7 +3297,7 @@
         <v>2.7E-4</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1.9100000000000001E-4</v>
       </c>
       <c r="F20">
         <v>1.3976499838110545E-4</v>
@@ -3306,7 +3317,7 @@
         <v>2.9E-4</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>2.5000000000000001E-4</v>
       </c>
       <c r="F21">
         <v>1.4862270528508646E-4</v>
@@ -3326,7 +3337,7 @@
         <v>3.2000000000000003E-4</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>4.3899999999999999E-4</v>
       </c>
       <c r="F22">
         <v>1.5719187650010074E-4</v>
@@ -3346,7 +3357,7 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>1.8599999999999999E-4</v>
       </c>
       <c r="F23">
         <v>1.6552960819378934E-4</v>
@@ -3366,7 +3377,7 @@
         <v>3.6000000000000002E-4</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>4.5300000000000001E-4</v>
       </c>
       <c r="F24">
         <v>1.7372582503532151E-4</v>
@@ -3386,7 +3397,7 @@
         <v>3.6999999999999999E-4</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1.1900000000000001E-4</v>
       </c>
       <c r="F25">
         <v>1.8190248848074241E-4</v>
@@ -3406,7 +3417,7 @@
         <v>3.8000000000000002E-4</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>2.9599999999999998E-4</v>
       </c>
       <c r="F26">
         <v>1.9021331496134574E-4</v>
@@ -3426,7 +3437,7 @@
         <v>3.8999999999999999E-4</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>1.45E-4</v>
       </c>
       <c r="F27">
         <v>1.9884453498457698E-4</v>
@@ -3446,7 +3457,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>1.4200000000000001E-4</v>
       </c>
       <c r="F28">
         <v>2.0801724018844521E-4</v>
@@ -3466,7 +3477,7 @@
         <v>4.0999999999999999E-4</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>3.3E-4</v>
       </c>
       <c r="F29">
         <v>2.1799191241094149E-4</v>
@@ -3486,7 +3497,7 @@
         <v>4.2999999999999999E-4</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>1.3300000000000001E-4</v>
       </c>
       <c r="F30">
         <v>2.2907582940519608E-4</v>
@@ -3506,7 +3517,7 @@
         <v>4.4999999999999999E-4</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>2.9100000000000003E-4</v>
       </c>
       <c r="F31">
         <v>2.4163422278563479E-4</v>
@@ -3526,7 +3537,7 @@
         <v>4.6999999999999999E-4</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>2.13E-4</v>
       </c>
       <c r="F32">
         <v>2.5610636024937469E-4</v>
@@ -3546,7 +3557,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>4.06E-4</v>
       </c>
       <c r="F33">
         <v>2.7296296629465634E-4</v>
@@ -3566,7 +3577,7 @@
         <v>5.1999999999999995E-4</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>3.3300000000000002E-4</v>
       </c>
       <c r="F34">
         <v>2.9250427707378537E-4</v>
@@ -3586,7 +3597,7 @@
         <v>5.4000000000000001E-4</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>4.5199999999999998E-4</v>
       </c>
       <c r="F35">
         <v>3.1501103482418474E-4</v>
@@ -3606,7 +3617,7 @@
         <v>5.5999999999999995E-4</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>3.7100000000000002E-4</v>
       </c>
       <c r="F36">
         <v>3.4080369634590497E-4</v>
@@ -3626,7 +3637,7 @@
         <v>5.6999999999999998E-4</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>3.4699999999999998E-4</v>
       </c>
       <c r="F37">
         <v>3.7024374991900219E-4</v>
@@ -3646,7 +3657,7 @@
         <v>5.9000000000000003E-4</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>4.06E-4</v>
       </c>
       <c r="F38">
         <v>4.0373464056616423E-4</v>
@@ -3666,7 +3677,7 @@
         <v>6.2E-4</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>3.77E-4</v>
       </c>
       <c r="F39">
         <v>4.4172202795553293E-4</v>
@@ -3686,7 +3697,7 @@
         <v>6.6E-4</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>3.5E-4</v>
       </c>
       <c r="F40">
         <v>4.84693052836706E-4</v>
@@ -3706,7 +3717,7 @@
         <v>7.1000000000000002E-4</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>3.8099999999999999E-4</v>
       </c>
       <c r="F41">
         <v>5.3317423477398376E-4</v>
@@ -3726,7 +3737,7 @@
         <v>7.6999999999999996E-4</v>
       </c>
       <c r="E42">
-        <v>1E-3</v>
+        <v>5.04E-4</v>
       </c>
       <c r="F42">
         <v>5.8772756928759213E-4</v>
@@ -3746,7 +3757,7 @@
         <v>8.4999999999999995E-4</v>
       </c>
       <c r="E43">
-        <v>1E-3</v>
+        <v>5.1199999999999998E-4</v>
       </c>
       <c r="F43">
         <v>6.4894434081127161E-4</v>
@@ -3766,7 +3777,7 @@
         <v>9.3999999999999997E-4</v>
       </c>
       <c r="E44">
-        <v>1E-3</v>
+        <v>7.2300000000000001E-4</v>
       </c>
       <c r="F44">
         <v>7.1743612514279013E-4</v>
@@ -3786,7 +3797,7 @@
         <v>1.0300000000000001E-3</v>
       </c>
       <c r="E45">
-        <v>1E-3</v>
+        <v>5.5699999999999999E-4</v>
       </c>
       <c r="F45">
         <v>7.9382242906268297E-4</v>
@@ -3806,7 +3817,7 @@
         <v>1.1299999999999999E-3</v>
       </c>
       <c r="E46">
-        <v>1E-3</v>
+        <v>5.9299999999999999E-4</v>
       </c>
       <c r="F46">
         <v>8.7871441511241542E-4</v>
@@ -3826,7 +3837,7 @@
         <v>1.24E-3</v>
       </c>
       <c r="E47">
-        <v>1E-3</v>
+        <v>1.111E-3</v>
       </c>
       <c r="F47">
         <v>9.7269419745729039E-4</v>
@@ -3846,7 +3857,7 @@
         <v>1.3500000000000001E-3</v>
       </c>
       <c r="E48">
-        <v>1E-3</v>
+        <v>6.5799999999999995E-4</v>
       </c>
       <c r="F48">
         <v>1.07628928295342E-3</v>
@@ -3866,7 +3877,7 @@
         <v>1.48E-3</v>
       </c>
       <c r="E49">
-        <v>1E-3</v>
+        <v>1.021E-3</v>
       </c>
       <c r="F49">
         <v>1.1899418832379532E-3</v>
@@ -3886,7 +3897,7 @@
         <v>1.6100000000000001E-3</v>
       </c>
       <c r="E50">
-        <v>1E-3</v>
+        <v>1.2409999999999999E-3</v>
       </c>
       <c r="F50">
         <v>1.313973051548628E-3</v>
@@ -3906,7 +3917,7 @@
         <v>1.75E-3</v>
       </c>
       <c r="E51">
-        <v>1E-3</v>
+        <v>1.238E-3</v>
       </c>
       <c r="F51">
         <v>1.4485419125008685E-3</v>
@@ -3926,7 +3937,7 @@
         <v>1.9E-3</v>
       </c>
       <c r="E52">
-        <v>1E-3</v>
+        <v>1.4469999999999999E-3</v>
       </c>
       <c r="F52">
         <v>1.5936006602526166E-3</v>
@@ -3946,7 +3957,7 @@
         <v>2.0600000000000002E-3</v>
       </c>
       <c r="E53">
-        <v>2E-3</v>
+        <v>1.72E-3</v>
       </c>
       <c r="F53">
         <v>1.7490875897062505E-3</v>
@@ -3966,7 +3977,7 @@
         <v>2.2399999999999998E-3</v>
       </c>
       <c r="E54">
-        <v>2E-3</v>
+        <v>1.897E-3</v>
       </c>
       <c r="F54">
         <v>1.9157838024795603E-3</v>
@@ -3986,7 +3997,7 @@
         <v>2.4399999999999999E-3</v>
       </c>
       <c r="E55">
-        <v>2E-3</v>
+        <v>1.673E-3</v>
       </c>
       <c r="F55">
         <v>2.0949007047471554E-3</v>
@@ -4006,7 +4017,7 @@
         <v>2.65E-3</v>
       </c>
       <c r="E56">
-        <v>2E-3</v>
+        <v>2.333E-3</v>
       </c>
       <c r="F56">
         <v>2.2879236172858343E-3</v>
@@ -4026,7 +4037,7 @@
         <v>2.8900000000000002E-3</v>
       </c>
       <c r="E57">
-        <v>2E-3</v>
+        <v>2.4220000000000001E-3</v>
       </c>
       <c r="F57">
         <v>2.4966626153897437E-3</v>
@@ -4046,7 +4057,7 @@
         <v>3.15E-3</v>
       </c>
       <c r="E58">
-        <v>3.0000000000000001E-3</v>
+        <v>2.627E-3</v>
       </c>
       <c r="F58">
         <v>2.7233131253591608E-3</v>
@@ -4066,7 +4077,7 @@
         <v>3.4399999999999999E-3</v>
       </c>
       <c r="E59">
-        <v>3.0000000000000001E-3</v>
+        <v>2.9420000000000002E-3</v>
       </c>
       <c r="F59">
         <v>2.9705290909114498E-3</v>
@@ -4086,7 +4097,7 @@
         <v>3.7599999999999999E-3</v>
       </c>
       <c r="E60">
-        <v>3.0000000000000001E-3</v>
+        <v>2.826E-3</v>
       </c>
       <c r="F60">
         <v>3.2415123149463474E-3</v>
@@ -4106,7 +4117,7 @@
         <v>4.1200000000000004E-3</v>
       </c>
       <c r="E61">
-        <v>3.0000000000000001E-3</v>
+        <v>3.1410000000000001E-3</v>
       </c>
       <c r="F61">
         <v>3.5401226030269549E-3</v>
@@ -4126,7 +4137,7 @@
         <v>4.5100000000000001E-3</v>
       </c>
       <c r="E62">
-        <v>3.0000000000000001E-3</v>
+        <v>3.0209999999999998E-3</v>
       </c>
       <c r="F62">
         <v>3.8710146661012595E-3</v>
@@ -4146,7 +4157,7 @@
         <v>4.9399999999999999E-3</v>
       </c>
       <c r="E63">
-        <v>4.0000000000000001E-3</v>
+        <v>4.4250000000000001E-3</v>
       </c>
       <c r="F63">
         <v>4.2398094926264741E-3</v>
@@ -4166,7 +4177,7 @@
         <v>5.4299999999999999E-3</v>
       </c>
       <c r="E64">
-        <v>5.0000000000000001E-3</v>
+        <v>5.1739999999999998E-3</v>
       </c>
       <c r="F64">
         <v>4.653310226976461E-3</v>
@@ -4186,7 +4197,7 @@
         <v>5.96E-3</v>
       </c>
       <c r="E65">
-        <v>6.0000000000000001E-3</v>
+        <v>5.9129999999999999E-3</v>
       </c>
       <c r="F65">
         <v>5.1197757022909208E-3</v>
@@ -4206,7 +4217,7 @@
         <v>6.5500000000000003E-3</v>
       </c>
       <c r="E66">
-        <v>5.0000000000000001E-3</v>
+        <v>5.3249999999999999E-3</v>
       </c>
       <c r="F66">
         <v>5.6492689638449256E-3</v>
@@ -4226,7 +4237,7 @@
         <v>7.2100000000000003E-3</v>
       </c>
       <c r="E67">
-        <v>7.0000000000000001E-3</v>
+        <v>6.7279999999999996E-3</v>
       </c>
       <c r="F67">
         <v>6.2541037915358486E-3</v>
@@ -4246,7 +4257,7 @@
         <v>7.9500000000000005E-3</v>
       </c>
       <c r="E68">
-        <v>7.0000000000000001E-3</v>
+        <v>6.8659999999999997E-3</v>
       </c>
       <c r="F68">
         <v>6.9486192807599201E-3</v>
@@ -4266,7 +4277,7 @@
         <v>8.7600000000000004E-3</v>
       </c>
       <c r="E69">
-        <v>8.0000000000000002E-3</v>
+        <v>7.6039999999999996E-3</v>
       </c>
       <c r="F69">
         <v>7.74678448930747E-3</v>
@@ -4286,7 +4297,7 @@
         <v>9.6799999999999994E-3</v>
       </c>
       <c r="E70">
-        <v>7.0000000000000001E-3</v>
+        <v>7.1329999999999996E-3</v>
       </c>
       <c r="F70">
         <v>8.6638882139277763E-3</v>
@@ -4306,7 +4317,7 @@
         <v>1.069E-2</v>
       </c>
       <c r="E71">
-        <v>0.01</v>
+        <v>9.8720000000000006E-3</v>
       </c>
       <c r="F71">
         <v>9.7174317364654757E-3</v>
@@ -4326,7 +4337,7 @@
         <v>1.183E-2</v>
       </c>
       <c r="E72">
-        <v>0.01</v>
+        <v>1.0153000000000001E-2</v>
       </c>
       <c r="F72">
         <v>1.092738722705203E-2</v>
@@ -4346,7 +4357,7 @@
         <v>1.3100000000000001E-2</v>
       </c>
       <c r="E73">
-        <v>1.2E-2</v>
+        <v>1.2393E-2</v>
       </c>
       <c r="F73">
         <v>1.2316469287713178E-2</v>
@@ -4366,7 +4377,7 @@
         <v>1.451E-2</v>
       </c>
       <c r="E74">
-        <v>1.4999999999999999E-2</v>
+        <v>1.4607E-2</v>
       </c>
       <c r="F74">
         <v>1.3910414383167279E-2</v>
@@ -4386,7 +4397,7 @@
         <v>1.61E-2</v>
       </c>
       <c r="E75">
-        <v>1.6E-2</v>
+        <v>1.6202000000000001E-2</v>
       </c>
       <c r="F75">
         <v>1.573826070364447E-2</v>
@@ -4406,7 +4417,7 @@
         <v>1.788E-2</v>
       </c>
       <c r="E76">
-        <v>1.6E-2</v>
+        <v>1.6188999999999999E-2</v>
       </c>
       <c r="F76">
         <v>1.7832618341325091E-2</v>
@@ -4426,7 +4437,7 @@
         <v>1.9879999999999998E-2</v>
       </c>
       <c r="E77">
-        <v>0.02</v>
+        <v>1.9536999999999999E-2</v>
       </c>
       <c r="F77">
         <v>2.0229916514965432E-2</v>
@@ -4446,7 +4457,7 @@
         <v>2.2120000000000001E-2</v>
       </c>
       <c r="E78">
-        <v>2.1000000000000001E-2</v>
+        <v>2.0618999999999998E-2</v>
       </c>
       <c r="F78">
         <v>2.2970610948685757E-2</v>
@@ -4466,7 +4477,7 @@
         <v>2.4639999999999999E-2</v>
       </c>
       <c r="E79">
-        <v>2.5000000000000001E-2</v>
+        <v>2.4938999999999999E-2</v>
       </c>
       <c r="F79">
         <v>2.6099330438751046E-2</v>
@@ -4486,7 +4497,7 @@
         <v>2.7470000000000001E-2</v>
       </c>
       <c r="E80">
-        <v>2.4E-2</v>
+        <v>2.4122000000000001E-2</v>
       </c>
       <c r="F80">
         <v>2.9664937213182349E-2</v>
@@ -4506,7 +4517,7 @@
         <v>3.066E-2</v>
       </c>
       <c r="E81">
-        <v>3.1E-2</v>
+        <v>3.1134999999999999E-2</v>
       </c>
       <c r="F81">
         <v>3.3720471052875498E-2</v>
@@ -4526,7 +4537,7 @@
         <v>3.4250000000000003E-2</v>
       </c>
       <c r="E82">
-        <v>3.3000000000000002E-2</v>
+        <v>3.3413999999999999E-2</v>
       </c>
       <c r="F82">
         <v>3.832294252727881E-2</v>
@@ -4546,7 +4557,7 @@
         <v>3.8300000000000001E-2</v>
       </c>
       <c r="E83">
-        <v>3.9E-2</v>
+        <v>3.8626000000000001E-2</v>
       </c>
       <c r="F83">
         <v>4.3532936422513893E-2</v>
@@ -4566,7 +4577,7 @@
         <v>4.2869999999999998E-2</v>
       </c>
       <c r="E84">
-        <v>4.3999999999999997E-2</v>
+        <v>4.3622000000000001E-2</v>
       </c>
       <c r="F84">
         <v>4.9413982929011488E-2</v>
@@ -4586,7 +4597,7 @@
         <v>4.8039999999999999E-2</v>
       </c>
       <c r="E85">
-        <v>5.1999999999999998E-2</v>
+        <v>5.2234000000000003E-2</v>
       </c>
       <c r="F85">
         <v>5.603165194388679E-2</v>
@@ -4606,7 +4617,7 @@
         <v>5.3879999999999997E-2</v>
       </c>
       <c r="E86">
-        <v>6.0999999999999999E-2</v>
+        <v>6.1438E-2</v>
       </c>
       <c r="F86">
         <v>6.3452325574084575E-2</v>
@@ -4626,7 +4637,7 @@
         <v>6.0490000000000002E-2</v>
       </c>
       <c r="E87">
-        <v>6.3E-2</v>
+        <v>6.3023999999999997E-2</v>
       </c>
       <c r="F87">
         <v>7.1741606339392014E-2</v>
@@ -4646,7 +4657,7 @@
         <v>6.7979999999999999E-2</v>
       </c>
       <c r="E88">
-        <v>7.3999999999999996E-2</v>
+        <v>7.3853000000000002E-2</v>
       </c>
       <c r="F88">
         <v>8.0962324476212363E-2</v>
@@ -4666,7 +4677,7 @@
         <v>7.6469999999999996E-2</v>
       </c>
       <c r="E89">
-        <v>8.5999999999999993E-2</v>
+        <v>8.5595000000000004E-2</v>
       </c>
       <c r="F89">
         <v>9.1172117958426835E-2</v>
@@ -4686,7 +4697,7 @@
         <v>8.6099999999999996E-2</v>
       </c>
       <c r="E90">
-        <v>0.10100000000000001</v>
+        <v>0.101086</v>
       </c>
       <c r="F90">
         <v>0.10242057415317013</v>
@@ -4706,7 +4717,7 @@
         <v>9.7049999999999997E-2</v>
       </c>
       <c r="E91">
-        <v>0.105</v>
+        <v>0.10517799999999999</v>
       </c>
       <c r="F91">
         <v>0.11474594304200567</v>
@@ -4726,7 +4737,7 @@
         <v>0.1095</v>
       </c>
       <c r="E92">
-        <v>0.127</v>
+        <v>0.12664600000000001</v>
       </c>
       <c r="F92">
         <v>0.12817145902143215</v>
@@ -4746,7 +4757,7 @@
         <v>0.12333</v>
       </c>
       <c r="E93">
-        <v>0.152</v>
+        <v>0.15173200000000001</v>
       </c>
       <c r="F93">
         <v>0.14270557561528044</v>
@@ -4766,7 +4777,7 @@
         <v>0.13830000000000001</v>
       </c>
       <c r="E94">
-        <v>0.158</v>
+        <v>0.15799299999999999</v>
       </c>
       <c r="F94">
         <v>0.15835416654300119</v>
@@ -4786,7 +4797,7 @@
         <v>0.15440000000000001</v>
       </c>
       <c r="E95">
-        <v>0.18</v>
+        <v>0.18001200000000001</v>
       </c>
       <c r="F95">
         <v>0.17511090322818437</v>
@@ -4806,7 +4817,7 @@
         <v>0.17161999999999999</v>
       </c>
       <c r="E96">
-        <v>0.19800000000000001</v>
+        <v>0.19849</v>
       </c>
       <c r="F96">
         <v>0.19295152804320315</v>
@@ -4826,7 +4837,7 @@
         <v>0.19103999999999999</v>
       </c>
       <c r="E97">
-        <v>0.22600000000000001</v>
+        <v>0.22561</v>
       </c>
       <c r="F97">
         <v>0.21183162495801186</v>
@@ -4846,7 +4857,7 @@
         <v>0.21045</v>
       </c>
       <c r="E98">
-        <v>0.26600000000000001</v>
+        <v>0.26590599999999998</v>
       </c>
       <c r="F98">
         <v>0.23168457214683438</v>
@@ -4866,7 +4877,7 @@
         <v>0.23088</v>
       </c>
       <c r="E99">
-        <v>0.29799999999999999</v>
+        <v>0.29788100000000001</v>
       </c>
       <c r="F99">
         <v>0.25241977490827655</v>
@@ -4906,7 +4917,7 @@
         <v>0.27422999999999997</v>
       </c>
       <c r="E101">
-        <v>0.312</v>
+        <v>0.31199900000000003</v>
       </c>
       <c r="F101">
         <v>0.2960469050617045</v>
@@ -4926,7 +4937,7 @@
         <v>0.29681000000000002</v>
       </c>
       <c r="E102">
-        <v>0.4</v>
+        <v>0.40027099999999999</v>
       </c>
       <c r="F102">
         <v>0.31862791122911427</v>
@@ -5339,10 +5350,318 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="17.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>17</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0.89</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.98546061111111116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>0.94</v>
+      </c>
+      <c r="E3">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="F3">
+        <v>0.879</v>
+      </c>
+      <c r="G3">
+        <v>0.87</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.97251985714285716</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>34</v>
+      </c>
+      <c r="D4">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="E4">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="F4">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="G4">
+        <v>0.87</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.93993930000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>44</v>
+      </c>
+      <c r="D5">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="E5">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.878</v>
+      </c>
+      <c r="G5">
+        <v>0.85</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.88740710000000012</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>45</v>
+      </c>
+      <c r="C6">
+        <v>54</v>
+      </c>
+      <c r="D6">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="E6">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="F6">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="G6">
+        <v>0.82</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.83289360000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>55</v>
+      </c>
+      <c r="C7">
+        <v>64</v>
+      </c>
+      <c r="D7">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="E7">
+        <v>0.83</v>
+      </c>
+      <c r="F7">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="G7">
+        <v>0.8</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.78203029999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>65</v>
+      </c>
+      <c r="C8">
+        <v>74</v>
+      </c>
+      <c r="D8">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="E8">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="F8">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="G8">
+        <v>0.8</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.73301919999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>75</v>
+      </c>
+      <c r="C9">
+        <v>200</v>
+      </c>
+      <c r="D9">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="E9">
+        <v>0.755</v>
+      </c>
+      <c r="F9">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="G9">
+        <v>0.76</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.69030099999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5375,255 +5694,6 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>17</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>0.89</v>
-      </c>
-      <c r="H2">
-        <v>0.98546061111111116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>24</v>
-      </c>
-      <c r="D3">
-        <v>0.94</v>
-      </c>
-      <c r="E3">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="F3">
-        <v>0.879</v>
-      </c>
-      <c r="G3">
-        <v>0.87</v>
-      </c>
-      <c r="H3">
-        <v>0.97251985714285716</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4">
-        <v>25</v>
-      </c>
-      <c r="C4">
-        <v>34</v>
-      </c>
-      <c r="D4">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="E4">
-        <v>0.91200000000000003</v>
-      </c>
-      <c r="F4">
-        <v>0.88100000000000001</v>
-      </c>
-      <c r="G4">
-        <v>0.87</v>
-      </c>
-      <c r="H4">
-        <v>0.93993930000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5">
-        <v>35</v>
-      </c>
-      <c r="C5">
-        <v>44</v>
-      </c>
-      <c r="D5">
-        <v>0.91100000000000003</v>
-      </c>
-      <c r="E5">
-        <v>0.88900000000000001</v>
-      </c>
-      <c r="F5">
-        <v>0.878</v>
-      </c>
-      <c r="G5">
-        <v>0.85</v>
-      </c>
-      <c r="H5">
-        <v>0.88740710000000012</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6">
-        <v>45</v>
-      </c>
-      <c r="C6">
-        <v>54</v>
-      </c>
-      <c r="D6">
-        <v>0.84699999999999998</v>
-      </c>
-      <c r="E6">
-        <v>0.85499999999999998</v>
-      </c>
-      <c r="F6">
-        <v>0.85499999999999998</v>
-      </c>
-      <c r="G6">
-        <v>0.82</v>
-      </c>
-      <c r="H6">
-        <v>0.83289360000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7">
-        <v>55</v>
-      </c>
-      <c r="C7">
-        <v>64</v>
-      </c>
-      <c r="D7">
-        <v>0.79900000000000004</v>
-      </c>
-      <c r="E7">
-        <v>0.83</v>
-      </c>
-      <c r="F7">
-        <v>0.83899999999999997</v>
-      </c>
-      <c r="G7">
-        <v>0.8</v>
-      </c>
-      <c r="H7">
-        <v>0.78203029999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8">
-        <v>65</v>
-      </c>
-      <c r="C8">
-        <v>74</v>
-      </c>
-      <c r="D8">
-        <v>0.77900000000000003</v>
-      </c>
-      <c r="E8">
-        <v>0.81699999999999995</v>
-      </c>
-      <c r="F8">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="G8">
-        <v>0.8</v>
-      </c>
-      <c r="H8">
-        <v>0.73301919999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9">
-        <v>75</v>
-      </c>
-      <c r="C9">
-        <v>200</v>
-      </c>
-      <c r="D9">
-        <v>0.72599999999999998</v>
-      </c>
-      <c r="E9">
-        <v>0.755</v>
-      </c>
-      <c r="F9">
-        <v>0.86099999999999999</v>
-      </c>
-      <c r="G9">
-        <v>0.76</v>
-      </c>
-      <c r="H9">
-        <v>0.69030099999999994</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2">
@@ -5881,6 +5951,13 @@
       <c r="H11">
         <v>0.24465116279069768</v>
       </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>